<commit_message>
Slight tweak to example data remove identifier
</commit_message>
<xml_diff>
--- a/example_data/example_rawdata.xlsx
+++ b/example_data/example_rawdata.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruybal.s/Documents/covid-19/covidClassifyR/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41D67D2-35DC-F445-95BC-84A458BEBBBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3DADFC-66A3-3240-B96B-ACF3E52011EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Covid-19 CSS_plate 7_20210513_0" sheetId="1" r:id="rId1"/>
+    <sheet name="Example plate" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1986,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>